<commit_message>
Validations & import fixes
</commit_message>
<xml_diff>
--- a/src/dbadmin/test.xlsx
+++ b/src/dbadmin/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="274" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="274" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>ID</t>
   </si>
@@ -39,6 +39,9 @@
     <t>DOM</t>
   </si>
   <si>
+    <t>LM</t>
+  </si>
+  <si>
     <t>ProductID</t>
   </si>
   <si>
@@ -60,6 +63,9 @@
     <t>Order Sourcing</t>
   </si>
   <si>
+    <t>Wilin' Out</t>
+  </si>
+  <si>
     <t>ModuleID</t>
   </si>
   <si>
@@ -81,6 +87,15 @@
     <t>Customer Order Sourcing</t>
   </si>
   <si>
+    <t>Claims</t>
+  </si>
+  <si>
+    <t>Detentions</t>
+  </si>
+  <si>
+    <t>Cost Allocation</t>
+  </si>
+  <si>
     <t>SystemAreaID</t>
   </si>
   <si>
@@ -120,10 +135,16 @@
     <t>Execute a full PO Import</t>
   </si>
   <si>
-    <t>Create Customer Order</t>
+    <t>create Customer Order</t>
   </si>
   <si>
     <t>Create a single Customer Order</t>
+  </si>
+  <si>
+    <t>Choo Choo!</t>
+  </si>
+  <si>
+    <t>Riding the train!</t>
   </si>
   <si>
     <t>KeyActionID</t>
@@ -237,10 +258,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -286,6 +307,16 @@
       </c>
       <c r="B5" s="0" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -304,10 +335,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -320,7 +351,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>1</v>
@@ -334,7 +365,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -345,7 +376,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -356,7 +387,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -367,7 +398,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -378,7 +409,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -389,7 +420,29 @@
         <v>4</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -408,10 +461,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -424,7 +477,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>1</v>
@@ -438,7 +491,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -449,18 +502,15 @@
         <v>2</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>3</v>
-      </c>
       <c r="C4" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -471,18 +521,15 @@
         <v>4</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>5</v>
-      </c>
       <c r="B6" s="0" t="n">
         <v>5</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -493,7 +540,40 @@
         <v>6</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -512,10 +592,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -531,16 +611,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -551,10 +631,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>0</v>
@@ -568,10 +648,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>0</v>
@@ -585,10 +665,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>0</v>
@@ -602,10 +682,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>0</v>
@@ -619,10 +699,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>0</v>
@@ -636,13 +716,24 @@
         <v>6</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -663,8 +754,8 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -677,7 +768,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>1</v>
@@ -691,7 +782,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -702,7 +793,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -713,7 +804,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -724,7 +815,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -735,7 +826,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>